<commit_message>
update table with open source column
</commit_message>
<xml_diff>
--- a/paper/previous_BH_NS_studies.xlsx
+++ b/paper/previous_BH_NS_studies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomwagg/Documents/detecting-DCOs-in-LISA/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA169E4-BC42-7D40-B2AF-8064F3E0348D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6988C807-4E6A-3143-9EAE-41199141D54D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{932AC085-5DF1-7346-88C0-42B7380C67FF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="74">
   <si>
     <t>Author</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>LISA Mission Time (years)</t>
+  </si>
+  <si>
+    <t>Open Source Code</t>
   </si>
 </sst>
 </file>
@@ -817,18 +820,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -905,15 +896,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
@@ -936,12 +918,58 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="77">
+    <dxf>
+      <font>
+        <color rgb="FF6D0605"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF8C81"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1003,24 +1031,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1118,9 +1129,6 @@
           <color rgb="FFFFFFFF"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1151,6 +1159,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thick">
@@ -1243,9 +1254,6 @@
           <color rgb="FFFFFFFF"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1276,13 +1284,114 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+        <left/>
+        <right style="thick">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
           <color theme="0"/>
         </left>
         <right/>
         <vertical/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1304,12 +1413,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thick">
@@ -1323,108 +1426,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
+        <left style="medium">
           <color theme="0"/>
         </left>
         <right/>
         <vertical/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color theme="0"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color theme="0"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color theme="0"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1503,28 +1511,28 @@
     <filterColumn colId="14" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{D5BF35A2-FB1D-6A49-9F0A-76B8FA65EB81}" name="Author" totalsRowLabel="Total" dataDxfId="46" totalsRowDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{E98E891B-5677-E14F-B7FD-6BEBF3F21A9A}" name="Year" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{06DDA78C-9D73-FF41-B9DB-B2F336F906AA}" name="BHBH" dataDxfId="47" totalsRowDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{DFC45EC4-2F0C-814E-8982-051696B2F68B}" name="BHNS" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{A240A617-F19A-B942-B652-48F4979F2291}" name="NSNS" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{A3381924-6772-7342-A5C9-D114C1823241}" name="Star formation history" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="8" xr3:uid="{C371F868-4A48-5840-B808-68E0684BE195}" name="Spatial distribution" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{DAEE09C4-384B-3E4D-9A96-E2000A449252}" name="Galactic Components" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{B6889DA3-EC68-6D4C-A262-97DE6D094611}" name="Metallicity Dependent Distributions" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{BB993792-72A2-1041-90ED-AE9230A7B456}" name="Code" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{9FB7A67B-118D-C348-BD48-F8CFDC9CA6F9}" name="Metallicity" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{266FE277-4F6F-9D44-9DDE-8ADC17509FF7}" name="Binary Physics Variations" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{0FE92553-561E-F149-9869-34BFC04DA351}" name="SNR Limit" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{D44A37E3-F2B2-5A44-8211-F5DA7CEA4BAD}" name="LISA Mission Time (yr)" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="16" xr3:uid="{8C0480D7-1E75-A44F-B432-A0DF655A21AE}" name="Eccentricity Treatment" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{D5BF35A2-FB1D-6A49-9F0A-76B8FA65EB81}" name="Author" totalsRowLabel="Total" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{E98E891B-5677-E14F-B7FD-6BEBF3F21A9A}" name="Year" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="6" xr3:uid="{06DDA78C-9D73-FF41-B9DB-B2F336F906AA}" name="BHBH" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{DFC45EC4-2F0C-814E-8982-051696B2F68B}" name="BHNS" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{A240A617-F19A-B942-B652-48F4979F2291}" name="NSNS" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{A3381924-6772-7342-A5C9-D114C1823241}" name="Star formation history" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{C371F868-4A48-5840-B808-68E0684BE195}" name="Spatial distribution" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{DAEE09C4-384B-3E4D-9A96-E2000A449252}" name="Galactic Components" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="10" xr3:uid="{B6889DA3-EC68-6D4C-A262-97DE6D094611}" name="Metallicity Dependent Distributions" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="11" xr3:uid="{BB993792-72A2-1041-90ED-AE9230A7B456}" name="Code" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{9FB7A67B-118D-C348-BD48-F8CFDC9CA6F9}" name="Metallicity" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{266FE277-4F6F-9D44-9DDE-8ADC17509FF7}" name="Binary Physics Variations" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="14" xr3:uid="{0FE92553-561E-F149-9869-34BFC04DA351}" name="SNR Limit" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="15" xr3:uid="{D44A37E3-F2B2-5A44-8211-F5DA7CEA4BAD}" name="LISA Mission Time (yr)" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="16" xr3:uid="{8C0480D7-1E75-A44F-B432-A0DF655A21AE}" name="Eccentricity Treatment" dataDxfId="47" totalsRowDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74235517-E93D-4140-BC61-628F9EAAA7F0}" name="Table42" displayName="Table42" ref="A2:I10" headerRowDxfId="45" dataDxfId="44" headerRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74235517-E93D-4140-BC61-628F9EAAA7F0}" name="Table42" displayName="Table42" ref="A2:I10" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44">
   <autoFilter ref="A2:I10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1537,23 +1545,23 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C16E36B3-7909-9140-95A0-C7B734EEB1E5}" name="Author" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{094CE8C4-D180-AB47-921C-07A582F1F0B8}" name="Year" dataDxfId="39" totalsRowDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{3B2DD959-7BCC-0A4B-8AE8-55885204793A}" name="BHBH" dataDxfId="37" totalsRowDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{C16E36B3-7909-9140-95A0-C7B734EEB1E5}" name="Author" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{094CE8C4-D180-AB47-921C-07A582F1F0B8}" name="Year" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{3B2DD959-7BCC-0A4B-8AE8-55885204793A}" name="BHBH" dataDxfId="38" totalsRowDxfId="37"/>
     <tableColumn id="5" xr3:uid="{2A2A6F2A-3208-A649-A62B-05AF0AB58E76}" name="BHNS" dataDxfId="36"/>
     <tableColumn id="4" xr3:uid="{67EC5ECB-8656-B349-BE6A-19FD3EE5C26D}" name="NSNS" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{92055AF3-8A92-FD47-8CB9-A7C5D983966F}" name="Star formation history" dataDxfId="33" totalsRowDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{8E7176E2-A165-B948-8409-E8383BBCA366}" name="Spatial distribution" dataDxfId="31" totalsRowDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{A17150A4-D6C6-E74A-83A4-7B388387BF8F}" name="Galactic Components" dataDxfId="29" totalsRowDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{EA2EF397-729D-834B-BB64-42995E6E87BC}" name="Metallicity Dependent Distributions" dataDxfId="27" totalsRowDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{92055AF3-8A92-FD47-8CB9-A7C5D983966F}" name="Star formation history" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{8E7176E2-A165-B948-8409-E8383BBCA366}" name="Spatial distribution" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{A17150A4-D6C6-E74A-83A4-7B388387BF8F}" name="Galactic Components" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{EA2EF397-729D-834B-BB64-42995E6E87BC}" name="Metallicity Dependent Distributions" dataDxfId="28" totalsRowDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F8CDD45-1369-874B-A0E2-47D889B0A69A}" name="Table423" displayName="Table423" ref="A2:H10" headerRowDxfId="26" dataDxfId="25" headerRowBorderDxfId="24">
-  <autoFilter ref="A2:H10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F8CDD45-1369-874B-A0E2-47D889B0A69A}" name="Table423" displayName="Table423" ref="A2:I10" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25">
+  <autoFilter ref="A2:I10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1562,16 +1570,18 @@
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C5516696-4302-864F-87CA-3BC4051AAAA0}" name="Author" totalsRowLabel="Total" dataDxfId="22" totalsRowDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{6F6E8470-AE29-B649-BC45-A036B2A6DCC7}" name="Year" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{937A5F1E-664C-6640-A400-C01732D20791}" name="Code" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{7BA3491D-92F6-D74E-A8C1-47600BE73E82}" name="Metallicity" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{6260072A-38BE-A747-91D4-1ECC109A52AA}" name="Binary Physics Variations" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{A452EB60-994F-DC44-83A1-A73289962BD8}" name="SNR Limit" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{60137873-8FC8-844F-9DAE-60662D0068B5}" name="LISA Mission Time (years)" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{FE63B066-19D3-9141-8B01-CD93E9DA232D}" name="Eccentricity Treatment" dataDxfId="8" totalsRowDxfId="9"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{C5516696-4302-864F-87CA-3BC4051AAAA0}" name="Author" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{6F6E8470-AE29-B649-BC45-A036B2A6DCC7}" name="Year" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{937A5F1E-664C-6640-A400-C01732D20791}" name="Code" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{4429DC09-7A2F-314D-A660-05919ACC0790}" name="Open Source Code" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{7BA3491D-92F6-D74E-A8C1-47600BE73E82}" name="Metallicity" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{6260072A-38BE-A747-91D4-1ECC109A52AA}" name="Binary Physics Variations" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{A452EB60-994F-DC44-83A1-A73289962BD8}" name="SNR Limit" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{60137873-8FC8-844F-9DAE-60662D0068B5}" name="LISA Mission Time (years)" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{FE63B066-19D3-9141-8B01-CD93E9DA232D}" name="Eccentricity Treatment" dataDxfId="9" totalsRowDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1901,29 +1911,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="51" t="s">
+      <c r="A1" s="48"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="21" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="21" t="s">
+      <c r="K1" s="55"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="23"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="56"/>
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1933,13 +1943,13 @@
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
@@ -1975,107 +1985,107 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" s="3" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="21">
         <v>2021</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="37">
+      <c r="L3" s="33">
         <v>15</v>
       </c>
-      <c r="M3" s="34">
+      <c r="M3" s="30">
         <v>7</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="37" t="s">
+      <c r="O3" s="33" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="36">
         <v>2020</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L4" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="37">
         <v>7</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="41" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="3" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="51" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="44">
         <v>93</v>
       </c>
       <c r="D5" s="3">
@@ -2116,13 +2126,13 @@
       </c>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="51" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="44" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -2163,13 +2173,13 @@
       </c>
     </row>
     <row r="7" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="51" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>2018</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="44">
         <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2210,13 +2220,13 @@
       </c>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="51" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="7">
         <v>2014</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="44">
         <v>6</v>
       </c>
       <c r="D8" s="3">
@@ -2257,13 +2267,13 @@
       </c>
     </row>
     <row r="9" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="51" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="7">
         <v>2010</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="44" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2299,54 +2309,54 @@
       <c r="N9" s="3">
         <v>1</v>
       </c>
-      <c r="O9" s="43" t="s">
+      <c r="O9" s="39" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="24">
         <v>2001</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="45">
         <v>0</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="25">
         <v>3</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>39</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="31">
+      <c r="K10" s="27">
         <v>0.02</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="25">
         <v>1</v>
       </c>
-      <c r="O10" s="33" t="s">
+      <c r="O10" s="29" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2395,7 +2405,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2412,20 +2422,20 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="51" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="24"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2435,13 +2445,13 @@
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
@@ -2459,71 +2469,71 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="21">
         <v>2021</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="36">
         <v>2020</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="51" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="44">
         <v>93</v>
       </c>
       <c r="D5" s="3">
@@ -2546,13 +2556,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="51" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="44" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -2575,13 +2585,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="51" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>2018</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="44">
         <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2604,13 +2614,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="51" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="7">
         <v>2014</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="44">
         <v>6</v>
       </c>
       <c r="D8" s="3">
@@ -2633,13 +2643,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="51" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="7">
         <v>2010</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="44" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2661,32 +2671,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="24">
         <v>2001</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="45">
         <v>0</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="25">
         <v>3</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>39</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="28" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2710,6 +2720,328 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C13 C7 C2:F5 D6:F10">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2508DF9F-E23B-2B4B-B19B-4C99EB93E90F}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="12.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="55"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="21">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="33">
+        <v>15</v>
+      </c>
+      <c r="G3" s="30">
+        <v>7</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="36">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="37">
+        <v>7</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="8">
+        <v>7</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="8">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2018</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="9">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2014</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="8">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2010</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="8">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="24">
+        <v>2001</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="25">
+        <v>1</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:D2 G2:G10 C3:C10">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2722,298 +3054,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2508DF9F-E23B-2B4B-B19B-4C99EB93E90F}">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="25">
-        <v>2021</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="37">
-        <v>15</v>
-      </c>
-      <c r="F3" s="34">
-        <v>7</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="40">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="41">
-        <v>7</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7">
-        <v>2020</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="8">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3">
-        <v>4</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7">
-        <v>2020</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="18">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="8">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3">
-        <v>4</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="7">
-        <v>2018</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="9">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3">
-        <v>4</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="7">
-        <v>2014</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="18">
-        <v>0.02</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="8">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="7">
-        <v>2010</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="8">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="28">
-        <v>2001</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="31">
-        <v>0.02</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="29">
-        <v>1</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E13"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C2:C10 F2:F10">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adjust spreadsheet with new galaxy
</commit_message>
<xml_diff>
--- a/paper/previous_BH_NS_studies.xlsx
+++ b/paper/previous_BH_NS_studies.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomwagg/Documents/detecting-DCOs-in-LISA/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6988C807-4E6A-3143-9EAE-41199141D54D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5FF0D8-E693-374B-A69D-C7FCC767514D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{932AC085-5DF1-7346-88C0-42B7380C67FF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{932AC085-5DF1-7346-88C0-42B7380C67FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="small1" sheetId="3" r:id="rId2"/>
-    <sheet name="small2" sheetId="4" r:id="rId3"/>
+    <sheet name="small1" sheetId="5" r:id="rId2"/>
+    <sheet name="small2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="77">
   <si>
     <t>Author</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Galactic Components</t>
   </si>
   <si>
-    <t>Thin disc</t>
-  </si>
-  <si>
     <t>LISA Mission Time (yr)</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Disc</t>
-  </si>
-  <si>
     <t>FIRE simulation</t>
   </si>
   <si>
@@ -140,15 +134,9 @@
     <t>Constant</t>
   </si>
   <si>
-    <t>Disc or halo</t>
-  </si>
-  <si>
     <t>Case BB always unstable, Single SN, alpha=0.1</t>
   </si>
   <si>
-    <t>Exponential, radially dependent</t>
-  </si>
-  <si>
     <t>4.2, 6.5</t>
   </si>
   <si>
@@ -179,9 +167,6 @@
     <t xml:space="preserve">50 bins between [1e-4, 3e-2] </t>
   </si>
   <si>
-    <t>Disc (thin + thick), bulge</t>
-  </si>
-  <si>
     <t>Liu</t>
   </si>
   <si>
@@ -218,15 +203,6 @@
     <t>4, 10</t>
   </si>
   <si>
-    <t>Exponential (Eq. 4)</t>
-  </si>
-  <si>
-    <t>Exponential radial, sech vertical (Eq. 5)</t>
-  </si>
-  <si>
-    <t>Constant over 10 Gyr (disc), 1 Gyr burst 10 Gyr ago (bulge), burst at 13 Gyr (halo)</t>
-  </si>
-  <si>
     <t>Exponential sphere (bulge), exponential radial and vertical (disc), spherical shell (halo)</t>
   </si>
   <si>
@@ -236,28 +212,70 @@
     <t>Constant over 13.7 Gyr</t>
   </si>
   <si>
-    <t>Exponential radial, sech vertical (Eq.13 based on Benacquista+2007)</t>
-  </si>
-  <si>
     <t xml:space="preserve">13 bins between [1e-4, 3e-2] </t>
   </si>
   <si>
-    <t>Miyamoto+Nagai potential (disc); Wilkinson &amp; Evans potential (halo)</t>
-  </si>
-  <si>
-    <t>Constant over 10 Gyr (thin disc), 1 Gyr burst 10 Gyr ago (bulge), 1 Gyr burst 11 Gyr (thick disc)</t>
-  </si>
-  <si>
-    <t>Frankel+2018 radial, McMillan 2011 vertical (disc)</t>
-  </si>
-  <si>
     <t>McMillan 2011</t>
   </si>
   <si>
-    <t>LISA Mission Time (years)</t>
-  </si>
-  <si>
     <t>Open Source Code</t>
+  </si>
+  <si>
+    <t>Constant over 10 Gyr (thin disc),
+1 Gyr burst 10 Gyr ago (bulge),
+1 Gyr burst 11 Gyr (thick disc)</t>
+  </si>
+  <si>
+    <t>Constant over 10 Gyr (disc),
+1 Gyr burst 10 Gyr ago (bulge),
+burst at 13 Gyr (halo)</t>
+  </si>
+  <si>
+    <t>Exponential radial, sech vertical (Benacquista+2007)</t>
+  </si>
+  <si>
+    <t>Exponential sphere (bulge),
+exponential radial and vertical (disc),
+spherical shell (halo)</t>
+  </si>
+  <si>
+    <t>Thin disc, thick disc, bulge</t>
+  </si>
+  <si>
+    <t>Exponential radial and vertical
+Different scale length and height for each component, thin disc has inside-out growth</t>
+  </si>
+  <si>
+    <t>Exponential over 10 Gyr</t>
+  </si>
+  <si>
+    <t>Exponential radial, sech^2 vertical</t>
+  </si>
+  <si>
+    <t>Exponential 8-0 Gyr ago (thin disc), Exponential 12-8 Gyr ago (thick disc), Skewed gaussian 0-6 Gyr (bulge)</t>
+  </si>
+  <si>
+    <t>Miyamoto &amp; Nagai potential (disc)
+Wilkinson &amp; Evans potential (halo)</t>
+  </si>
+  <si>
+    <t>Single disc</t>
+  </si>
+  <si>
+    <t>Single disc or halo</t>
+  </si>
+  <si>
+    <t>LISA Mission Time</t>
+  </si>
+  <si>
+    <t>Exponential radial and vertical, scale length/height for each component, thin disc has inside-out growth</t>
+  </si>
+  <si>
+    <t>Miyamoto &amp; Nagai potential (disc), Wilkinson &amp; Evans potential (halo)</t>
+  </si>
+  <si>
+    <t>Exponential radial,
+sech^2 vertical</t>
   </si>
 </sst>
 </file>
@@ -350,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -742,10 +760,108 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="0"/>
       </left>
       <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
         <color theme="0"/>
       </right>
       <top/>
@@ -758,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -853,9 +969,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -916,35 +1029,340 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="91">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF6D0605"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF8C81"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF6D0605"/>
@@ -971,64 +1389,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <vertical/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1048,70 +1428,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color theme="0"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color theme="0"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color theme="0"/>
@@ -1129,6 +1445,9 @@
           <color rgb="FFFFFFFF"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1161,26 +1480,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF6D0605"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF8C81"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right style="thick">
+        <right style="thin">
           <color theme="0"/>
         </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
         <vertical/>
+        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1192,7 +1528,10 @@
           <color theme="0"/>
         </left>
         <right/>
+        <top/>
+        <bottom/>
         <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1254,6 +1593,9 @@
           <color rgb="FFFFFFFF"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1284,6 +1626,137 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF6D0605"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF8C81"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF6D0605"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF8C81"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF6D0605"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF8C81"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1303,59 +1776,11 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color theme="0"/>
         </left>
         <right/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color theme="0"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color theme="0"/>
-        </right>
         <vertical/>
       </border>
     </dxf>
@@ -1492,8 +1917,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D1C5A5B4-5491-F84E-B0A3-0F84177ABE79}" name="Table4" displayName="Table4" ref="A2:O10" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75">
-  <autoFilter ref="A2:O10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D1C5A5B4-5491-F84E-B0A3-0F84177ABE79}" name="Table4" displayName="Table4" ref="A2:P10" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89">
+  <autoFilter ref="A2:P10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1509,30 +1934,32 @@
     <filterColumn colId="12" hiddenButton="1"/>
     <filterColumn colId="13" hiddenButton="1"/>
     <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{D5BF35A2-FB1D-6A49-9F0A-76B8FA65EB81}" name="Author" totalsRowLabel="Total" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{E98E891B-5677-E14F-B7FD-6BEBF3F21A9A}" name="Year" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{06DDA78C-9D73-FF41-B9DB-B2F336F906AA}" name="BHBH" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{DFC45EC4-2F0C-814E-8982-051696B2F68B}" name="BHNS" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{A240A617-F19A-B942-B652-48F4979F2291}" name="NSNS" dataDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{A3381924-6772-7342-A5C9-D114C1823241}" name="Star formation history" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{C371F868-4A48-5840-B808-68E0684BE195}" name="Spatial distribution" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{DAEE09C4-384B-3E4D-9A96-E2000A449252}" name="Galactic Components" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="10" xr3:uid="{B6889DA3-EC68-6D4C-A262-97DE6D094611}" name="Metallicity Dependent Distributions" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="11" xr3:uid="{BB993792-72A2-1041-90ED-AE9230A7B456}" name="Code" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="12" xr3:uid="{9FB7A67B-118D-C348-BD48-F8CFDC9CA6F9}" name="Metallicity" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{266FE277-4F6F-9D44-9DDE-8ADC17509FF7}" name="Binary Physics Variations" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="14" xr3:uid="{0FE92553-561E-F149-9869-34BFC04DA351}" name="SNR Limit" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="15" xr3:uid="{D44A37E3-F2B2-5A44-8211-F5DA7CEA4BAD}" name="LISA Mission Time (yr)" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="16" xr3:uid="{8C0480D7-1E75-A44F-B432-A0DF655A21AE}" name="Eccentricity Treatment" dataDxfId="47" totalsRowDxfId="46"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{D5BF35A2-FB1D-6A49-9F0A-76B8FA65EB81}" name="Author" totalsRowLabel="Total" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{E98E891B-5677-E14F-B7FD-6BEBF3F21A9A}" name="Year" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{06DDA78C-9D73-FF41-B9DB-B2F336F906AA}" name="BHBH" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{DFC45EC4-2F0C-814E-8982-051696B2F68B}" name="BHNS" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{A240A617-F19A-B942-B652-48F4979F2291}" name="NSNS" dataDxfId="80"/>
+    <tableColumn id="11" xr3:uid="{BB993792-72A2-1041-90ED-AE9230A7B456}" name="Code" dataDxfId="62" totalsRowDxfId="66"/>
+    <tableColumn id="12" xr3:uid="{9FB7A67B-118D-C348-BD48-F8CFDC9CA6F9}" name="Open Source Code" dataDxfId="61" totalsRowDxfId="65"/>
+    <tableColumn id="13" xr3:uid="{266FE277-4F6F-9D44-9DDE-8ADC17509FF7}" name="Metallicity" dataDxfId="60" totalsRowDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{869FF47B-D99B-CB45-97D7-FDD50768598B}" name="Binary Physics Variations" dataDxfId="59" totalsRowDxfId="63"/>
+    <tableColumn id="7" xr3:uid="{A3381924-6772-7342-A5C9-D114C1823241}" name="Star formation history" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{C371F868-4A48-5840-B808-68E0684BE195}" name="Spatial distribution" dataDxfId="68" totalsRowDxfId="77"/>
+    <tableColumn id="9" xr3:uid="{DAEE09C4-384B-3E4D-9A96-E2000A449252}" name="Galactic Components" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="10" xr3:uid="{B6889DA3-EC68-6D4C-A262-97DE6D094611}" name="Metallicity Dependent Distributions" dataDxfId="67" totalsRowDxfId="74"/>
+    <tableColumn id="14" xr3:uid="{0FE92553-561E-F149-9869-34BFC04DA351}" name="SNR Limit" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="15" xr3:uid="{D44A37E3-F2B2-5A44-8211-F5DA7CEA4BAD}" name="LISA Mission Time (yr)" dataDxfId="58" totalsRowDxfId="71"/>
+    <tableColumn id="16" xr3:uid="{8C0480D7-1E75-A44F-B432-A0DF655A21AE}" name="Eccentricity Treatment" dataDxfId="70" totalsRowDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74235517-E93D-4140-BC61-628F9EAAA7F0}" name="Table42" displayName="Table42" ref="A2:I10" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C044637-D768-6F4F-AD9B-78AE98191DB5}" name="Table42" displayName="Table42" ref="A2:I10" headerRowDxfId="57" dataDxfId="56" headerRowBorderDxfId="55">
   <autoFilter ref="A2:I10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1545,22 +1972,22 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C16E36B3-7909-9140-95A0-C7B734EEB1E5}" name="Author" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{094CE8C4-D180-AB47-921C-07A582F1F0B8}" name="Year" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{3B2DD959-7BCC-0A4B-8AE8-55885204793A}" name="BHBH" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{2A2A6F2A-3208-A649-A62B-05AF0AB58E76}" name="BHNS" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{67EC5ECB-8656-B349-BE6A-19FD3EE5C26D}" name="NSNS" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{92055AF3-8A92-FD47-8CB9-A7C5D983966F}" name="Star formation history" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{8E7176E2-A165-B948-8409-E8383BBCA366}" name="Spatial distribution" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{A17150A4-D6C6-E74A-83A4-7B388387BF8F}" name="Galactic Components" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{EA2EF397-729D-834B-BB64-42995E6E87BC}" name="Metallicity Dependent Distributions" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{44BDF58C-D579-1240-8E39-C70254FC8FD5}" name="Author" totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{BB0F4036-7566-224F-83E6-E99475C68172}" name="Year" dataDxfId="51" totalsRowDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{0B5424FA-9670-BE4A-8FBE-933CAF9BDEC7}" name="BHBH" dataDxfId="49" totalsRowDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{99449272-02BF-8C40-B571-0FE9CB6AABE2}" name="BHNS" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{10E711C6-591C-0A4E-9A91-BB52D008A09A}" name="NSNS" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{123E8E5E-4F6E-934F-B285-7B85EFE6D228}" name="Code" dataDxfId="45" totalsRowDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{FDCA272B-6B76-9F48-81F1-722F6E83ADAC}" name="Open Source Code" dataDxfId="43" totalsRowDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{374386BD-013A-3747-A3A9-B61786C5680A}" name="Metallicity" dataDxfId="41" totalsRowDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{FC99DA5E-D174-D140-B921-4B5ECCBC1832}" name="Binary Physics Variations" dataDxfId="0" totalsRowDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F8CDD45-1369-874B-A0E2-47D889B0A69A}" name="Table423" displayName="Table423" ref="A2:I10" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA01D837-27BE-BF40-B1B8-DA80E55E2DA0}" name="Table43" displayName="Table43" ref="A2:I10" headerRowDxfId="39" dataDxfId="38" headerRowBorderDxfId="37">
   <autoFilter ref="A2:I10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1573,15 +2000,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C5516696-4302-864F-87CA-3BC4051AAAA0}" name="Author" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{6F6E8470-AE29-B649-BC45-A036B2A6DCC7}" name="Year" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{937A5F1E-664C-6640-A400-C01732D20791}" name="Code" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{4429DC09-7A2F-314D-A660-05919ACC0790}" name="Open Source Code" dataDxfId="0" totalsRowDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{7BA3491D-92F6-D74E-A8C1-47600BE73E82}" name="Metallicity" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{6260072A-38BE-A747-91D4-1ECC109A52AA}" name="Binary Physics Variations" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{A452EB60-994F-DC44-83A1-A73289962BD8}" name="SNR Limit" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{60137873-8FC8-844F-9DAE-60662D0068B5}" name="LISA Mission Time (years)" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{FE63B066-19D3-9141-8B01-CD93E9DA232D}" name="Eccentricity Treatment" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{A59F038C-9360-6A40-836A-1F712AB9CDD8}" name="Author" totalsRowLabel="Total" dataDxfId="35" totalsRowDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{31074774-FA7B-3847-A5DF-05A38C3AD9E4}" name="Year" dataDxfId="33" totalsRowDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{651801BA-D8D0-2D47-A1E5-CC2E0B2B5408}" name="Star formation history" dataDxfId="31" totalsRowDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{77A1DBA9-110E-D444-A279-2C730A46719A}" name="Spatial distribution" dataDxfId="29" totalsRowDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{72C3BA5C-69B1-8F46-A599-EE28E3A3F6B0}" name="Galactic Components" dataDxfId="27" totalsRowDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{98AFBC29-35E5-C847-BEAF-728294FC965A}" name="Metallicity Dependent Distributions" dataDxfId="25" totalsRowDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{264FAE28-5817-E14F-BE99-CA3E693777BB}" name="SNR Limit" dataDxfId="23" totalsRowDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{7317F1AC-9096-5648-9404-B10BA000E023}" name="LISA Mission Time" dataDxfId="21" totalsRowDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{F659EE55-08CC-4945-91BA-BF9725B6ACAD}" name="Eccentricity Treatment" dataDxfId="1" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1884,7 +2311,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E912B5E-7704-CF4C-915A-9DB9BFA3D958}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <selection sqref="A1:I10"/>
@@ -1897,46 +2324,51 @@
     <col min="3" max="3" width="9.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18.6640625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="12.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.1640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10" style="2" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="54" t="s">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="55"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="5"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="3" customFormat="1" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1953,139 +2385,148 @@
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1"/>
+      <c r="O2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:16" s="3" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:17" s="3" customFormat="1" ht="69" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="21">
         <v>2021</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="65">
+        <v>15</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="66">
+        <v>7</v>
+      </c>
+      <c r="O3" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="35">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="30" t="s">
+      <c r="I4" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="33">
-        <v>15</v>
-      </c>
-      <c r="M3" s="30">
+      <c r="N4" s="62">
         <v>7</v>
       </c>
-      <c r="N3" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>29</v>
+      <c r="O4" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="40" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="36">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="37">
-        <v>7</v>
-      </c>
-      <c r="N4" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:17" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="50" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="43">
         <v>93</v>
       </c>
       <c r="D5" s="3">
@@ -2095,138 +2536,147 @@
         <v>8</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>47</v>
+        <v>16</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="62">
+        <v>7</v>
+      </c>
+      <c r="O5" s="62">
+        <v>4</v>
+      </c>
+      <c r="P5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="8">
-        <v>7</v>
-      </c>
-      <c r="N5" s="3">
-        <v>4</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:17" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>41</v>
+      <c r="C6" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3">
         <v>35</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="18">
+      <c r="G6" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="18">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="L6" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="8">
+      <c r="I6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="62">
         <v>8</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="62">
         <v>4</v>
       </c>
-      <c r="O6" s="16" t="s">
-        <v>29</v>
+      <c r="P6" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:17" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>2018</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="43">
         <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>24</v>
+      <c r="G7" s="62" t="s">
+        <v>36</v>
       </c>
       <c r="H7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="9">
+      <c r="J7" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="62">
         <v>5</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="62">
         <v>4</v>
       </c>
-      <c r="O7" s="20" t="s">
-        <v>30</v>
+      <c r="P7" s="20" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
-        <v>48</v>
+    <row r="8" spans="1:17" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="50" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="7">
         <v>2014</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="43">
         <v>6</v>
       </c>
       <c r="D8" s="3">
@@ -2236,91 +2686,97 @@
         <v>16</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0.02</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="18">
-        <v>0.02</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="8">
+        <v>25</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" s="62">
         <v>7</v>
       </c>
-      <c r="N8" s="3">
+      <c r="O8" s="63">
         <v>2</v>
       </c>
-      <c r="O8" s="17" t="s">
-        <v>64</v>
+      <c r="P8" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
-        <v>49</v>
+    <row r="9" spans="1:17" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="50" t="s">
+        <v>44</v>
       </c>
       <c r="B9" s="7">
         <v>2010</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="J9" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" s="8">
+      <c r="K9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="62">
         <v>10</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="63">
         <v>1</v>
       </c>
-      <c r="O9" s="39" t="s">
-        <v>29</v>
+      <c r="P9" s="38" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="24">
         <v>2001</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="44">
         <v>0</v>
       </c>
       <c r="D10" s="25">
@@ -2330,66 +2786,86 @@
         <v>39</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="G10" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0.02</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="27">
-        <v>0.02</v>
-      </c>
-      <c r="L10" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="63">
+        <v>1</v>
+      </c>
+      <c r="P10" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" s="25">
-        <v>1</v>
-      </c>
-      <c r="O10" s="29" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="L13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P6">
     <sortCondition ref="B3:B6"/>
   </sortState>
   <mergeCells count="4">
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="J1:M1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C13 C7 C2:F5 D6:F10 J2:J10 M2:M10">
-    <cfRule type="cellIs" dxfId="7" priority="23" operator="equal">
+  <conditionalFormatting sqref="C13 C7 C2:I5 D6:I10 N2">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G2 F3:F10">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2401,11 +2877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F00300E-14B0-6A4B-9487-64F8B43EC56E}">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4ACDD4-7DEA-874C-8A03-CA824D816CFA}">
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2415,30 +2891,33 @@
     <col min="3" max="3" width="9.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="12.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="60"/>
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="76"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2455,85 +2934,86 @@
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I2" s="70" t="s">
+        <v>39</v>
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="21">
         <v>2021</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="74">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="35">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>40</v>
-      </c>
+      <c r="I4" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4"/>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="36">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="50" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="43">
         <v>93</v>
       </c>
       <c r="D5" s="3">
@@ -2543,84 +3023,84 @@
         <v>8</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>41</v>
       </c>
+      <c r="I5" s="63" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>41</v>
+      <c r="C6" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3">
         <v>35</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>41</v>
+        <v>13</v>
+      </c>
+      <c r="G6" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="18">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="I6" s="73" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>2018</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="43">
         <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>24</v>
+      <c r="G7" s="62" t="s">
+        <v>36</v>
       </c>
       <c r="H7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
-        <v>48</v>
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="50" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="7">
         <v>2014</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="43">
         <v>6</v>
       </c>
       <c r="D8" s="3">
@@ -2630,55 +3110,55 @@
         <v>16</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>41</v>
+        <v>24</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="I8" s="63" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
-        <v>49</v>
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="50" t="s">
+        <v>44</v>
       </c>
       <c r="B9" s="7">
         <v>2010</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="24">
         <v>2001</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="44">
         <v>0</v>
       </c>
       <c r="D10" s="25">
@@ -2688,42 +3168,48 @@
         <v>39</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>41</v>
+        <v>14</v>
+      </c>
+      <c r="G10" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="H13"/>
+      <c r="I13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C13 C7 C2:F5 D6:F10">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="C13 C7 C2:I5 D6:I10">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G2 F3:F10">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2735,43 +3221,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2508DF9F-E23B-2B4B-B19B-4C99EB93E90F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E487B9-ECF3-544E-9164-F556514993CA}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="12.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="32.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="56"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2779,273 +3269,287 @@
         <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>28</v>
+        <v>73</v>
+      </c>
+      <c r="I2" s="70" t="s">
+        <v>26</v>
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="69" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="21">
         <v>2021</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="33">
-        <v>15</v>
-      </c>
-      <c r="G3" s="30">
+      <c r="C3" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="66">
         <v>7</v>
       </c>
-      <c r="H3" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>29</v>
+      <c r="H3" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="50" t="s">
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="35">
         <v>2020</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="37">
+        <v>22</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="62">
         <v>7</v>
       </c>
-      <c r="H4" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="41" t="s">
-        <v>30</v>
+      <c r="H4" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="71" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="50" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>45</v>
+      <c r="C5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="F5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="62">
+        <v>7</v>
+      </c>
+      <c r="H5" s="62">
+        <v>4</v>
+      </c>
+      <c r="I5" s="72" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" s="8">
-        <v>7</v>
-      </c>
-      <c r="H5" s="3">
-        <v>4</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="18">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="C6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="62">
         <v>8</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="62">
         <v>4</v>
       </c>
-      <c r="I6" s="16" t="s">
-        <v>29</v>
+      <c r="I6" s="72" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>2018</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>40</v>
+      <c r="C7" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="9">
+        <v>23</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="62">
         <v>5</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="62">
         <v>4</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>30</v>
+      <c r="I7" s="73" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
-        <v>48</v>
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="50" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="7">
         <v>2014</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="18">
-        <v>0.02</v>
+      <c r="C8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="8">
+        <v>37</v>
+      </c>
+      <c r="G8" s="62">
         <v>7</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="63">
         <v>2</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>64</v>
+      <c r="I8" s="63" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
-        <v>49</v>
+    <row r="9" spans="1:10" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="50" t="s">
+        <v>44</v>
       </c>
       <c r="B9" s="7">
         <v>2010</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="C9" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="8">
+      <c r="E9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="62">
         <v>10</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="63">
         <v>1</v>
       </c>
-      <c r="I9" s="39" t="s">
-        <v>29</v>
+      <c r="I9" s="62" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="24">
         <v>2001</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="27">
-        <v>0.02</v>
-      </c>
-      <c r="F10" s="28" t="s">
+      <c r="C10" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="68">
+        <v>1</v>
+      </c>
+      <c r="I10" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="25">
-        <v>1</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>29</v>
-      </c>
+      <c r="J10" s="69"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F13"/>
+      <c r="C13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:D2 G2:G10 C3:C10">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="G2">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add commands make things consistent, update table
</commit_message>
<xml_diff>
--- a/paper/previous_BH_NS_studies.xlsx
+++ b/paper/previous_BH_NS_studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomwagg/Documents/detecting-DCOs-in-LISA/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651A635F-C0B2-8C41-AFE5-B2D294AFF3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D19EBA-B3C3-BF4A-8EA6-D8EAD325109C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{932AC085-5DF1-7346-88C0-42B7380C67FF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20280" windowHeight="18000" xr2:uid="{932AC085-5DF1-7346-88C0-42B7380C67FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
   <si>
     <t>Author</t>
   </si>
@@ -189,15 +189,6 @@
   </si>
   <si>
     <t>Optimistic CE, Pessimistic CE</t>
-  </si>
-  <si>
-    <t>11.3, 19.3</t>
-  </si>
-  <si>
-    <t>26.7, 44.5</t>
-  </si>
-  <si>
-    <t>25.9, 42.0</t>
   </si>
   <si>
     <t>4, 10</t>
@@ -231,32 +222,13 @@
 burst at 13 Gyr (halo)</t>
   </si>
   <si>
-    <t>Exponential radial, sech vertical (Benacquista+2007)</t>
-  </si>
-  <si>
-    <t>Exponential sphere (bulge),
-exponential radial and vertical (disc),
-spherical shell (halo)</t>
-  </si>
-  <si>
     <t>Thin disc, thick disc, bulge</t>
   </si>
   <si>
-    <t>Exponential radial and vertical
-Different scale length and height for each component, thin disc has inside-out growth</t>
-  </si>
-  <si>
     <t>Exponential over 10 Gyr</t>
   </si>
   <si>
-    <t>Exponential radial, sech^2 vertical</t>
-  </si>
-  <si>
     <t>Exponential 8-0 Gyr ago (thin disc), Exponential 12-8 Gyr ago (thick disc), Skewed gaussian 0-6 Gyr (bulge)</t>
-  </si>
-  <si>
-    <t>Miyamoto &amp; Nagai potential (disc)
-Wilkinson &amp; Evans potential (halo)</t>
   </si>
   <si>
     <t>Single disc</t>
@@ -279,6 +251,15 @@
   </si>
   <si>
     <t>Exponential radial, sech^2 vertical (Benacquista+2007)</t>
+  </si>
+  <si>
+    <t>35.7, 56.3</t>
+  </si>
+  <si>
+    <t>32.8, 55.1</t>
+  </si>
+  <si>
+    <t>8.4, 13.5</t>
   </si>
 </sst>
 </file>
@@ -1113,6 +1094,49 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -1485,46 +1509,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1587,9 +1571,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1907,19 +1888,19 @@
     <tableColumn id="13" xr3:uid="{266FE277-4F6F-9D44-9DDE-8ADC17509FF7}" name="Metallicity" dataDxfId="65" totalsRowDxfId="64"/>
     <tableColumn id="3" xr3:uid="{869FF47B-D99B-CB45-97D7-FDD50768598B}" name="Binary Physics Variations" dataDxfId="63" totalsRowDxfId="62"/>
     <tableColumn id="7" xr3:uid="{A3381924-6772-7342-A5C9-D114C1823241}" name="Star formation history" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{C371F868-4A48-5840-B808-68E0684BE195}" name="Spatial distribution" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{DAEE09C4-384B-3E4D-9A96-E2000A449252}" name="Galactic Components" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{B6889DA3-EC68-6D4C-A262-97DE6D094611}" name="Metallicity Dependent Distributions" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="14" xr3:uid="{0FE92553-561E-F149-9869-34BFC04DA351}" name="SNR Limit" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="15" xr3:uid="{D44A37E3-F2B2-5A44-8211-F5DA7CEA4BAD}" name="LISA Mission Time (yr)" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="16" xr3:uid="{8C0480D7-1E75-A44F-B432-A0DF655A21AE}" name="Eccentricity Treatment" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{C371F868-4A48-5840-B808-68E0684BE195}" name="Spatial distribution" dataDxfId="0" totalsRowDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{DAEE09C4-384B-3E4D-9A96-E2000A449252}" name="Galactic Components" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{B6889DA3-EC68-6D4C-A262-97DE6D094611}" name="Metallicity Dependent Distributions" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="14" xr3:uid="{0FE92553-561E-F149-9869-34BFC04DA351}" name="SNR Limit" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="15" xr3:uid="{D44A37E3-F2B2-5A44-8211-F5DA7CEA4BAD}" name="LISA Mission Time (yr)" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="16" xr3:uid="{8C0480D7-1E75-A44F-B432-A0DF655A21AE}" name="Eccentricity Treatment" dataDxfId="50" totalsRowDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C044637-D768-6F4F-AD9B-78AE98191DB5}" name="Table42" displayName="Table42" ref="A2:I10" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C044637-D768-6F4F-AD9B-78AE98191DB5}" name="Table42" displayName="Table42" ref="A2:I10" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47">
   <autoFilter ref="A2:I10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1932,22 +1913,36 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{44BDF58C-D579-1240-8E39-C70254FC8FD5}" name="Author" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{BB0F4036-7566-224F-83E6-E99475C68172}" name="Year" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{0B5424FA-9670-BE4A-8FBE-933CAF9BDEC7}" name="BHBH" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{99449272-02BF-8C40-B571-0FE9CB6AABE2}" name="BHNS" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{10E711C6-591C-0A4E-9A91-BB52D008A09A}" name="NSNS" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{123E8E5E-4F6E-934F-B285-7B85EFE6D228}" name="Code" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{FDCA272B-6B76-9F48-81F1-722F6E83ADAC}" name="Open Source Code" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{374386BD-013A-3747-A3A9-B61786C5680A}" name="Metallicity" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{FC99DA5E-D174-D140-B921-4B5ECCBC1832}" name="Binary Physics Variations" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{44BDF58C-D579-1240-8E39-C70254FC8FD5}" name="Author" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{BB0F4036-7566-224F-83E6-E99475C68172}" name="Year" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{0B5424FA-9670-BE4A-8FBE-933CAF9BDEC7}" name="BHBH" dataDxfId="41" totalsRowDxfId="40">
+      <calculatedColumnFormula>Table4[[#This Row],[BHBH]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{99449272-02BF-8C40-B571-0FE9CB6AABE2}" name="BHNS" dataDxfId="39">
+      <calculatedColumnFormula>Table4[[#This Row],[BHNS]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{10E711C6-591C-0A4E-9A91-BB52D008A09A}" name="NSNS" dataDxfId="38">
+      <calculatedColumnFormula>Table4[[#This Row],[NSNS]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{123E8E5E-4F6E-934F-B285-7B85EFE6D228}" name="Code" dataDxfId="37" totalsRowDxfId="36">
+      <calculatedColumnFormula>Table4[[#This Row],[Code]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{FDCA272B-6B76-9F48-81F1-722F6E83ADAC}" name="Open Source Code" dataDxfId="35" totalsRowDxfId="34">
+      <calculatedColumnFormula>Table4[[#This Row],[Open Source Code]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{374386BD-013A-3747-A3A9-B61786C5680A}" name="Metallicity" dataDxfId="33" totalsRowDxfId="32">
+      <calculatedColumnFormula>Table4[[#This Row],[Metallicity]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{FC99DA5E-D174-D140-B921-4B5ECCBC1832}" name="Binary Physics Variations" dataDxfId="31" totalsRowDxfId="30">
+      <calculatedColumnFormula>Table4[[#This Row],[Binary Physics Variations]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA01D837-27BE-BF40-B1B8-DA80E55E2DA0}" name="Table43" displayName="Table43" ref="A2:I10" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA01D837-27BE-BF40-B1B8-DA80E55E2DA0}" name="Table43" displayName="Table43" ref="A2:I10" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24">
   <autoFilter ref="A2:I10" xr:uid="{D1F23B23-2B7B-B14A-B22D-BE517C88CFE3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1960,15 +1955,29 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A59F038C-9360-6A40-836A-1F712AB9CDD8}" name="Author" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{31074774-FA7B-3847-A5DF-05A38C3AD9E4}" name="Year" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{651801BA-D8D0-2D47-A1E5-CC2E0B2B5408}" name="Star formation history" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{77A1DBA9-110E-D444-A279-2C730A46719A}" name="Spatial distribution" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{72C3BA5C-69B1-8F46-A599-EE28E3A3F6B0}" name="Galactic Components" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{98AFBC29-35E5-C847-BEAF-728294FC965A}" name="Metallicity Dependent Distributions" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{264FAE28-5817-E14F-BE99-CA3E693777BB}" name="SNR Limit" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{7317F1AC-9096-5648-9404-B10BA000E023}" name="LISA Mission Time" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{F659EE55-08CC-4945-91BA-BF9725B6ACAD}" name="Eccentricity Treatment" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A59F038C-9360-6A40-836A-1F712AB9CDD8}" name="Author" totalsRowLabel="Total" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{31074774-FA7B-3847-A5DF-05A38C3AD9E4}" name="Year" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{651801BA-D8D0-2D47-A1E5-CC2E0B2B5408}" name="Star formation history" dataDxfId="18" totalsRowDxfId="17">
+      <calculatedColumnFormula>Table4[[#This Row],[Star formation history]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{77A1DBA9-110E-D444-A279-2C730A46719A}" name="Spatial distribution" dataDxfId="16" totalsRowDxfId="15">
+      <calculatedColumnFormula>Table4[[#This Row],[Spatial distribution]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{72C3BA5C-69B1-8F46-A599-EE28E3A3F6B0}" name="Galactic Components" dataDxfId="14" totalsRowDxfId="13">
+      <calculatedColumnFormula>Table4[[#This Row],[Galactic Components]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{98AFBC29-35E5-C847-BEAF-728294FC965A}" name="Metallicity Dependent Distributions" dataDxfId="12" totalsRowDxfId="11">
+      <calculatedColumnFormula>Table4[[#This Row],[Metallicity Dependent Distributions]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{264FAE28-5817-E14F-BE99-CA3E693777BB}" name="SNR Limit" dataDxfId="10" totalsRowDxfId="9">
+      <calculatedColumnFormula>Table4[[#This Row],[SNR Limit]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{7317F1AC-9096-5648-9404-B10BA000E023}" name="LISA Mission Time" dataDxfId="8" totalsRowDxfId="7">
+      <calculatedColumnFormula>Table4[[#This Row],[LISA Mission Time (yr)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{F659EE55-08CC-4945-91BA-BF9725B6ACAD}" name="Eccentricity Treatment" dataDxfId="6" totalsRowDxfId="5">
+      <calculatedColumnFormula>Table4[[#This Row],[Eccentricity Treatment]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2273,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E912B5E-7704-CF4C-915A-9DB9BFA3D958}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection sqref="A1:I10"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2348,7 +2357,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>30</v>
@@ -2387,13 +2396,13 @@
         <v>2021</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>13</v>
@@ -2405,16 +2414,16 @@
         <v>42</v>
       </c>
       <c r="I3" s="58">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J3" s="52" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K3" s="31" t="s">
         <v>66</v>
       </c>
       <c r="L3" s="52" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M3" s="32" t="s">
         <v>36</v>
@@ -2423,7 +2432,7 @@
         <v>7</v>
       </c>
       <c r="O3" s="53" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P3" s="32" t="s">
         <v>27</v>
@@ -2452,7 +2461,7 @@
         <v>36</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I4" s="39" t="s">
         <v>25</v>
@@ -2473,7 +2482,7 @@
         <v>7</v>
       </c>
       <c r="O4" s="55" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P4" s="40" t="s">
         <v>28</v>
@@ -2508,13 +2517,13 @@
         <v>25</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M5" s="17" t="s">
         <v>37</v>
@@ -2561,10 +2570,10 @@
         <v>31</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="M6" s="17" t="s">
         <v>37</v>
@@ -2602,7 +2611,7 @@
         <v>36</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>25</v>
@@ -2658,13 +2667,13 @@
         <v>25</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>71</v>
       </c>
       <c r="M8" s="17" t="s">
         <v>37</v>
@@ -2676,10 +2685,10 @@
         <v>2</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="50" t="s">
         <v>44</v>
       </c>
@@ -2708,10 +2717,10 @@
         <v>50</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>48</v>
@@ -2758,13 +2767,13 @@
         <v>25</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K10" s="25" t="s">
         <v>68</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="M10" s="28" t="s">
         <v>37</v>
@@ -2841,7 +2850,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2877,7 +2886,7 @@
       <c r="I1" s="71"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2897,7 +2906,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>30</v>
@@ -2907,237 +2916,293 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="21">
         <v>2021</v>
       </c>
-      <c r="C3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>42</v>
+      <c r="C3" s="41" t="str">
+        <f>Table4[[#This Row],[BHBH]]</f>
+        <v>35.7, 56.3</v>
+      </c>
+      <c r="D3" s="41" t="str">
+        <f>Table4[[#This Row],[BHNS]]</f>
+        <v>32.8, 55.1</v>
+      </c>
+      <c r="E3" s="41" t="str">
+        <f>Table4[[#This Row],[NSNS]]</f>
+        <v>8.4, 13.5</v>
+      </c>
+      <c r="F3" s="41" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>COMPAS</v>
+      </c>
+      <c r="G3" s="53" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✓</v>
+      </c>
+      <c r="H3" s="33" t="str">
+        <f>Table4[[#This Row],[Metallicity]]</f>
+        <v xml:space="preserve">50 bins between [1e-4, 3e-2] </v>
       </c>
       <c r="I3" s="66">
-        <v>15</v>
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="35">
         <v>2020</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="61" t="s">
-        <v>25</v>
+      <c r="C4" s="41" t="str">
+        <f>Table4[[#This Row],[BHBH]]</f>
+        <v>4.2, 6.5</v>
+      </c>
+      <c r="D4" s="41" t="str">
+        <f>Table4[[#This Row],[BHNS]]</f>
+        <v>✗</v>
+      </c>
+      <c r="E4" s="41" t="str">
+        <f>Table4[[#This Row],[NSNS]]</f>
+        <v>✗</v>
+      </c>
+      <c r="F4" s="36" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>BSE</v>
+      </c>
+      <c r="G4" s="54" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✓</v>
+      </c>
+      <c r="H4" s="15" t="str">
+        <f>Table4[[#This Row],[Metallicity]]</f>
+        <v xml:space="preserve">13 bins between [1e-4, 3e-2] </v>
+      </c>
+      <c r="I4" s="61" t="str">
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>None</v>
       </c>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="41">
+        <f>Table4[[#This Row],[BHBH]]</f>
         <v>93</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="41">
+        <f>Table4[[#This Row],[BHNS]]</f>
         <v>33</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="41">
+        <f>Table4[[#This Row],[NSNS]]</f>
         <v>8</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>25</v>
+      <c r="F5" s="8" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>COSMIC</v>
+      </c>
+      <c r="G5" s="54" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✓</v>
+      </c>
+      <c r="H5" s="19" t="str">
+        <f>Table4[[#This Row],[Metallicity]]</f>
+        <v>0.02, 0.003</v>
+      </c>
+      <c r="I5" s="56" t="str">
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>None</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="C6" s="41" t="str">
+        <f>Table4[[#This Row],[BHBH]]</f>
+        <v>✗</v>
+      </c>
+      <c r="D6" s="41" t="str">
+        <f>Table4[[#This Row],[BHNS]]</f>
+        <v>✗</v>
+      </c>
+      <c r="E6" s="41">
+        <f>Table4[[#This Row],[NSNS]]</f>
         <v>35</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="55" t="s">
-        <v>36</v>
+      <c r="F6" s="8" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>COMPAS</v>
+      </c>
+      <c r="G6" s="55" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✓</v>
       </c>
       <c r="H6" s="18">
+        <f>Table4[[#This Row],[Metallicity]]</f>
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="I6" s="65" t="s">
-        <v>32</v>
+      <c r="I6" s="65" t="str">
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>Case BB always unstable, Single SN, alpha=0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>2018</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="41">
+        <f>Table4[[#This Row],[BHBH]]</f>
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="56" t="s">
-        <v>25</v>
+      <c r="D7" s="41" t="str">
+        <f>Table4[[#This Row],[BHNS]]</f>
+        <v>✗</v>
+      </c>
+      <c r="E7" s="41" t="str">
+        <f>Table4[[#This Row],[NSNS]]</f>
+        <v>✗</v>
+      </c>
+      <c r="F7" s="9" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>BSE</v>
+      </c>
+      <c r="G7" s="55" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✓</v>
+      </c>
+      <c r="H7" s="15" t="str">
+        <f>Table4[[#This Row],[Metallicity]]</f>
+        <v xml:space="preserve">13 bins between [1e-4, 3e-2] </v>
+      </c>
+      <c r="I7" s="56" t="str">
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>None</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="7">
         <v>2014</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="41">
+        <f>Table4[[#This Row],[BHBH]]</f>
         <v>6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="41">
+        <f>Table4[[#This Row],[BHNS]]</f>
         <v>3</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="41">
+        <f>Table4[[#This Row],[NSNS]]</f>
         <v>16</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="55" t="s">
-        <v>36</v>
+      <c r="F8" s="8" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>BSE</v>
+      </c>
+      <c r="G8" s="55" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✓</v>
       </c>
       <c r="H8" s="18">
+        <f>Table4[[#This Row],[Metallicity]]</f>
         <v>0.02</v>
       </c>
-      <c r="I8" s="56" t="s">
-        <v>25</v>
+      <c r="I8" s="56" t="str">
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>None</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="7">
         <v>2010</v>
       </c>
-      <c r="C9" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="65" t="s">
-        <v>50</v>
+      <c r="C9" s="41" t="str">
+        <f>Table4[[#This Row],[BHBH]]</f>
+        <v>2.3, 0</v>
+      </c>
+      <c r="D9" s="41" t="str">
+        <f>Table4[[#This Row],[BHNS]]</f>
+        <v>0.2, 0</v>
+      </c>
+      <c r="E9" s="41" t="str">
+        <f>Table4[[#This Row],[NSNS]]</f>
+        <v>4, 1.7</v>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>Startrack</v>
+      </c>
+      <c r="G9" s="56" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✗</v>
+      </c>
+      <c r="H9" s="19" t="str">
+        <f>Table4[[#This Row],[Metallicity]]</f>
+        <v>0.02 (disc, bulge), 0.001 (halo)</v>
+      </c>
+      <c r="I9" s="65" t="str">
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>Optimistic CE, Pessimistic CE</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="24">
         <v>2001</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="41">
+        <f>Table4[[#This Row],[BHBH]]</f>
         <v>0</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="41">
+        <f>Table4[[#This Row],[BHNS]]</f>
         <v>3</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="41">
+        <f>Table4[[#This Row],[NSNS]]</f>
         <v>39</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>37</v>
+      <c r="F10" s="26" t="str">
+        <f>Table4[[#This Row],[Code]]</f>
+        <v>SeBa</v>
+      </c>
+      <c r="G10" s="57" t="str">
+        <f>Table4[[#This Row],[Open Source Code]]</f>
+        <v>✗</v>
       </c>
       <c r="H10" s="27">
+        <f>Table4[[#This Row],[Metallicity]]</f>
         <v>0.02</v>
       </c>
-      <c r="I10" s="57" t="s">
-        <v>25</v>
+      <c r="I10" s="57" t="str">
+        <f>Table4[[#This Row],[Binary Physics Variations]]</f>
+        <v>None</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -3157,19 +3222,19 @@
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C13 C7 C2:I5 D6:I10">
-    <cfRule type="cellIs" dxfId="47" priority="5" operator="equal">
+  <conditionalFormatting sqref="C13 C2:I10">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2 F3:F10">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3184,8 +3249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E487B9-ECF3-544E-9164-F556514993CA}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3244,7 +3309,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="I2" s="62" t="s">
         <v>26</v>
@@ -3258,26 +3323,33 @@
       <c r="B3" s="21">
         <v>2021</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>36</v>
+      <c r="C3" s="52" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>Exponential 8-0 Gyr ago (thin disc), Exponential 12-8 Gyr ago (thick disc), Skewed gaussian 0-6 Gyr (bulge)</v>
+      </c>
+      <c r="D3" s="31" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>Exponential radial and vertical, scale length/height for each component, thin disc has inside-out growth</v>
+      </c>
+      <c r="E3" s="52" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Thin disc, thick disc, bulge</v>
+      </c>
+      <c r="F3" s="32" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✓</v>
       </c>
       <c r="G3" s="59">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
         <v>7</v>
       </c>
-      <c r="H3" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>27</v>
+      <c r="H3" s="53" t="str">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
+        <v>4, 10</v>
+      </c>
+      <c r="I3" s="53" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Full</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -3287,26 +3359,33 @@
       <c r="B4" s="35">
         <v>2020</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>36</v>
+      <c r="C4" s="37" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>FIRE simulation</v>
+      </c>
+      <c r="D4" s="34" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>FIRE simulation</v>
+      </c>
+      <c r="E4" s="37" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Everything within 300kpc</v>
+      </c>
+      <c r="F4" s="38" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✓</v>
       </c>
       <c r="G4" s="55">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
         <v>7</v>
       </c>
-      <c r="H4" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="63" t="s">
-        <v>28</v>
+      <c r="H4" s="55" t="str">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
+        <v>4, 10</v>
+      </c>
+      <c r="I4" s="63" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Used for evolution, ignored during detection</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3316,26 +3395,35 @@
       <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>37</v>
+      <c r="C5" s="19" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>Constant over 10 Gyr (thin disc),
+1 Gyr burst 10 Gyr ago (bulge),
+1 Gyr burst 11 Gyr (thick disc)</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>McMillan 2011</v>
+      </c>
+      <c r="E5" s="15" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Thin disc, thick disc, bulge</v>
+      </c>
+      <c r="F5" s="17" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✗</v>
       </c>
       <c r="G5" s="55">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
         <v>7</v>
       </c>
       <c r="H5" s="55">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
         <v>4</v>
       </c>
-      <c r="I5" s="64" t="s">
-        <v>27</v>
+      <c r="I5" s="64" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Full</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3345,26 +3433,33 @@
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>37</v>
+      <c r="C6" s="18" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>Constant</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>Miyamoto &amp; Nagai potential (disc), Wilkinson &amp; Evans potential (halo)</v>
+      </c>
+      <c r="E6" s="19" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Single disc or halo</v>
+      </c>
+      <c r="F6" s="17" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✗</v>
       </c>
       <c r="G6" s="55">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
         <v>8</v>
       </c>
       <c r="H6" s="55">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
         <v>4</v>
       </c>
-      <c r="I6" s="64" t="s">
-        <v>27</v>
+      <c r="I6" s="64" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Full</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -3374,26 +3469,33 @@
       <c r="B7" s="7">
         <v>2018</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>36</v>
+      <c r="C7" s="37" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>FIRE simulation</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>FIRE simulation</v>
+      </c>
+      <c r="E7" s="15" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Everything within 300kpc</v>
+      </c>
+      <c r="F7" s="16" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✓</v>
       </c>
       <c r="G7" s="60">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
         <v>5</v>
       </c>
       <c r="H7" s="55">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
         <v>4</v>
       </c>
-      <c r="I7" s="65" t="s">
-        <v>28</v>
+      <c r="I7" s="65" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Used for evolution, ignored during detection</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -3403,26 +3505,33 @@
       <c r="B8" s="7">
         <v>2014</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>37</v>
+      <c r="C8" s="18" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>Constant over 13.7 Gyr</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>Exponential radial, sech^2 vertical (Benacquista+2007)</v>
+      </c>
+      <c r="E8" s="18" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Single disc</v>
+      </c>
+      <c r="F8" s="17" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✗</v>
       </c>
       <c r="G8" s="55">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
         <v>7</v>
       </c>
       <c r="H8" s="56">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
         <v>2</v>
       </c>
-      <c r="I8" s="56" t="s">
-        <v>56</v>
+      <c r="I8" s="56" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Assumed circular</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
@@ -3432,26 +3541,35 @@
       <c r="B9" s="7">
         <v>2010</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>37</v>
+      <c r="C9" s="19" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>Constant over 10 Gyr (disc),
+1 Gyr burst 10 Gyr ago (bulge),
+burst at 13 Gyr (halo)</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>Exponential sphere (bulge), exponential radial and vertical (disc), spherical shell (halo)</v>
+      </c>
+      <c r="E9" s="15" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Disc, bulge, halo</v>
+      </c>
+      <c r="F9" s="17" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✗</v>
       </c>
       <c r="G9" s="55">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
         <v>10</v>
       </c>
       <c r="H9" s="56">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
         <v>1</v>
       </c>
-      <c r="I9" s="55" t="s">
-        <v>27</v>
+      <c r="I9" s="55" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Full</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -3461,26 +3579,34 @@
       <c r="B10" s="24">
         <v>2001</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="60" t="s">
-        <v>40</v>
+      <c r="C10" s="19" t="str">
+        <f>Table4[[#This Row],[Star formation history]]</f>
+        <v>Exponential over 10 Gyr</v>
+      </c>
+      <c r="D10" s="25" t="str">
+        <f>Table4[[#This Row],[Spatial distribution]]</f>
+        <v>Exponential radial,
+sech^2 vertical</v>
+      </c>
+      <c r="E10" s="18" t="str">
+        <f>Table4[[#This Row],[Galactic Components]]</f>
+        <v>Single disc</v>
+      </c>
+      <c r="F10" s="39" t="str">
+        <f>Table4[[#This Row],[Metallicity Dependent Distributions]]</f>
+        <v>✗</v>
+      </c>
+      <c r="G10" s="60" t="str">
+        <f>Table4[[#This Row],[SNR Limit]]</f>
+        <v>1, 5</v>
       </c>
       <c r="H10" s="61">
+        <f>Table4[[#This Row],[LISA Mission Time (yr)]]</f>
         <v>1</v>
       </c>
-      <c r="I10" s="55" t="s">
-        <v>27</v>
+      <c r="I10" s="55" t="str">
+        <f>Table4[[#This Row],[Eccentricity Treatment]]</f>
+        <v>Full</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -3499,18 +3625,18 @@
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix table (SeBa is open source!)
</commit_message>
<xml_diff>
--- a/paper/previous_BH_NS_studies.xlsx
+++ b/paper/previous_BH_NS_studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomwagg/Documents/detecting-DCOs-in-LISA/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D0B1D1-25B1-E047-8543-E5463BA8D0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013399A9-04A3-AF45-9C08-496EF2FA30AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{932AC085-5DF1-7346-88C0-42B7380C67FF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{932AC085-5DF1-7346-88C0-42B7380C67FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="75">
   <si>
     <t>Year</t>
   </si>
@@ -617,39 +617,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,6 +634,39 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B16AE5-3AD4-7C4E-8D34-C7C8DDD88A3B}">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="A2" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,31 +1028,31 @@
     <row r="1" spans="1:22" s="4" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
       <c r="B1" s="26"/>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="37" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="37" t="s">
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="37" t="s">
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
       <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:22" s="12" customFormat="1" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1062,18 +1062,18 @@
       <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38" t="s">
+      <c r="F2" s="40"/>
+      <c r="G2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="39"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="29" t="s">
         <v>20</v>
       </c>
@@ -1116,22 +1116,22 @@
       <c r="B3" s="16">
         <v>2021</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="38" t="s">
         <v>73</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -1175,18 +1175,18 @@
       <c r="B4" s="17">
         <v>2021</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="44">
         <v>12</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36">
+      <c r="D4" s="45"/>
+      <c r="E4" s="45">
         <v>2</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="33" t="s">
+      <c r="F4" s="45"/>
+      <c r="G4" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="19" t="s">
         <v>23</v>
       </c>
@@ -1228,18 +1228,18 @@
       <c r="B5" s="17">
         <v>2020</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="42">
         <v>93</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42">
         <v>33</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33">
+      <c r="F5" s="42"/>
+      <c r="G5" s="42">
         <v>8</v>
       </c>
-      <c r="H5" s="34"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="12" t="s">
         <v>15</v>
       </c>
@@ -1281,18 +1281,18 @@
       <c r="B6" s="17">
         <v>2020</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33" t="s">
+      <c r="D6" s="42"/>
+      <c r="E6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33">
+      <c r="F6" s="42"/>
+      <c r="G6" s="42">
         <v>35</v>
       </c>
-      <c r="H6" s="34"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1341,14 +1341,14 @@
       <c r="D7" s="31">
         <v>6.5</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33" t="s">
+      <c r="F7" s="42"/>
+      <c r="G7" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="34"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="12" t="s">
         <v>23</v>
       </c>
@@ -1390,18 +1390,18 @@
       <c r="B8" s="17">
         <v>2018</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="42">
         <v>25</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33" t="s">
+      <c r="D8" s="42"/>
+      <c r="E8" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33" t="s">
+      <c r="F8" s="42"/>
+      <c r="G8" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="34"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1443,18 +1443,18 @@
       <c r="B9" s="17">
         <v>2014</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="42">
         <v>6</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33">
+      <c r="D9" s="42"/>
+      <c r="E9" s="42">
         <v>3</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33">
+      <c r="F9" s="42"/>
+      <c r="G9" s="42">
         <v>16</v>
       </c>
-      <c r="H9" s="34"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="12" t="s">
         <v>23</v>
       </c>
@@ -1555,23 +1555,23 @@
       <c r="B11" s="17">
         <v>2001</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="42">
         <v>0</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33">
+      <c r="D11" s="42"/>
+      <c r="E11" s="42">
         <v>3</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33">
+      <c r="F11" s="42"/>
+      <c r="G11" s="42">
         <v>39</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="43"/>
       <c r="I11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="23" t="s">
-        <v>33</v>
+      <c r="J11" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="K11" s="23">
         <v>0.02</v>
@@ -1876,13 +1876,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
@@ -1897,12 +1896,13 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:H11">
     <cfRule type="colorScale" priority="7">
@@ -1928,8 +1928,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1957,22 +1957,22 @@
         <f>'Sheet1 (2)'!B1</f>
         <v>0</v>
       </c>
-      <c r="C1" s="37" t="str">
+      <c r="C1" s="39" t="str">
         <f>'Sheet1 (2)'!C1</f>
         <v>Predicted DCO Detection Rates</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="37" t="str">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="39" t="str">
         <f>'Sheet1 (2)'!I1</f>
         <v>Population Synthesis</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="39"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1984,21 +1984,21 @@
         <f>'Sheet1 (2)'!B2</f>
         <v>Year</v>
       </c>
-      <c r="C2" s="41" t="str">
+      <c r="C2" s="47" t="str">
         <f>'Sheet1 (2)'!C2</f>
         <v>BHBH</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42" t="str">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48" t="str">
         <f>'Sheet1 (2)'!E2</f>
         <v>BHNS</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42" t="str">
+      <c r="F2" s="48"/>
+      <c r="G2" s="48" t="str">
         <f>'Sheet1 (2)'!G2</f>
         <v>NSNS</v>
       </c>
-      <c r="H2" s="43"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="29" t="str">
         <f>'Sheet1 (2)'!I2</f>
         <v>Code</v>
@@ -2026,27 +2026,27 @@
         <f>'Sheet1 (2)'!B3</f>
         <v>2021</v>
       </c>
-      <c r="C3" s="44" t="str">
+      <c r="C3" s="33" t="str">
         <f>'Sheet1 (2)'!C3</f>
         <v>6-154</v>
       </c>
-      <c r="D3" s="45" t="str">
+      <c r="D3" s="34" t="str">
         <f>'Sheet1 (2)'!D3</f>
         <v>9-238</v>
       </c>
-      <c r="E3" s="46" t="str">
+      <c r="E3" s="35" t="str">
         <f>'Sheet1 (2)'!E3</f>
         <v>2-198</v>
       </c>
-      <c r="F3" s="47" t="str">
+      <c r="F3" s="36" t="str">
         <f>'Sheet1 (2)'!F3</f>
         <v>3-289</v>
       </c>
-      <c r="G3" s="48" t="str">
+      <c r="G3" s="37" t="str">
         <f>'Sheet1 (2)'!G3</f>
         <v>3-35</v>
       </c>
-      <c r="H3" s="49" t="str">
+      <c r="H3" s="38" t="str">
         <f>'Sheet1 (2)'!H3</f>
         <v>4-57</v>
       </c>
@@ -2076,21 +2076,21 @@
         <f>'Sheet1 (2)'!B4</f>
         <v>2021</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="44">
         <f>'Sheet1 (2)'!C4</f>
         <v>12</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36">
+      <c r="D4" s="45"/>
+      <c r="E4" s="45">
         <f>'Sheet1 (2)'!E4</f>
         <v>2</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="33" t="str">
+      <c r="F4" s="45"/>
+      <c r="G4" s="42" t="str">
         <f>'Sheet1 (2)'!G4</f>
         <v>✗</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="19" t="str">
         <f>'Sheet1 (2)'!I4</f>
         <v>BSE</v>
@@ -2117,21 +2117,21 @@
         <f>'Sheet1 (2)'!B5</f>
         <v>2020</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="46">
         <f>'Sheet1 (2)'!C5</f>
         <v>93</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42">
         <f>'Sheet1 (2)'!E5</f>
         <v>33</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33">
+      <c r="F5" s="42"/>
+      <c r="G5" s="42">
         <f>'Sheet1 (2)'!G5</f>
         <v>8</v>
       </c>
-      <c r="H5" s="34"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="12" t="str">
         <f>'Sheet1 (2)'!I5</f>
         <v>COSMIC</v>
@@ -2158,21 +2158,21 @@
         <f>'Sheet1 (2)'!B6</f>
         <v>2020</v>
       </c>
-      <c r="C6" s="40" t="str">
+      <c r="C6" s="46" t="str">
         <f>'Sheet1 (2)'!C6</f>
         <v>✗</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33" t="str">
+      <c r="D6" s="42"/>
+      <c r="E6" s="42" t="str">
         <f>'Sheet1 (2)'!E6</f>
         <v>✗</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33">
+      <c r="F6" s="42"/>
+      <c r="G6" s="42">
         <f>'Sheet1 (2)'!G6</f>
         <v>35</v>
       </c>
-      <c r="H6" s="34"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="12" t="str">
         <f>'Sheet1 (2)'!I6</f>
         <v>COMPAS</v>
@@ -2207,16 +2207,16 @@
         <f>'Sheet1 (2)'!D7</f>
         <v>6.5</v>
       </c>
-      <c r="E7" s="33" t="str">
+      <c r="E7" s="42" t="str">
         <f>'Sheet1 (2)'!E7</f>
         <v>✗</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33" t="str">
+      <c r="F7" s="42"/>
+      <c r="G7" s="42" t="str">
         <f>'Sheet1 (2)'!G7</f>
         <v>✗</v>
       </c>
-      <c r="H7" s="34"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="12" t="str">
         <f>'Sheet1 (2)'!I7</f>
         <v>BSE</v>
@@ -2243,21 +2243,21 @@
         <f>'Sheet1 (2)'!B8</f>
         <v>2018</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="46">
         <f>'Sheet1 (2)'!C8</f>
         <v>25</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33" t="str">
+      <c r="D8" s="42"/>
+      <c r="E8" s="42" t="str">
         <f>'Sheet1 (2)'!E8</f>
         <v>✗</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33" t="str">
+      <c r="F8" s="42"/>
+      <c r="G8" s="42" t="str">
         <f>'Sheet1 (2)'!G8</f>
         <v>✗</v>
       </c>
-      <c r="H8" s="34"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="7" t="str">
         <f>'Sheet1 (2)'!I8</f>
         <v>BSE</v>
@@ -2284,21 +2284,21 @@
         <f>'Sheet1 (2)'!B9</f>
         <v>2014</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="46">
         <f>'Sheet1 (2)'!C9</f>
         <v>6</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33">
+      <c r="D9" s="42"/>
+      <c r="E9" s="42">
         <f>'Sheet1 (2)'!E9</f>
         <v>3</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33">
+      <c r="F9" s="42"/>
+      <c r="G9" s="42">
         <f>'Sheet1 (2)'!G9</f>
         <v>16</v>
       </c>
-      <c r="H9" s="34"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="12" t="str">
         <f>'Sheet1 (2)'!I9</f>
         <v>BSE</v>
@@ -2375,28 +2375,27 @@
         <f>'Sheet1 (2)'!B11</f>
         <v>2001</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="46">
         <f>'Sheet1 (2)'!C11</f>
         <v>0</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33">
+      <c r="D11" s="42"/>
+      <c r="E11" s="42">
         <f>'Sheet1 (2)'!E11</f>
         <v>3</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33">
+      <c r="F11" s="42"/>
+      <c r="G11" s="42">
         <f>'Sheet1 (2)'!G11</f>
         <v>39</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="43"/>
       <c r="I11" s="12" t="str">
         <f>'Sheet1 (2)'!I11</f>
         <v>SeBa</v>
       </c>
-      <c r="J11" s="30" t="str">
-        <f>'Sheet1 (2)'!J11</f>
-        <v>✗</v>
+      <c r="J11" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="K11" s="30">
         <f>'Sheet1 (2)'!K11</f>
@@ -2517,15 +2516,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
@@ -2542,6 +2532,15 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:H11">
     <cfRule type="colorScale" priority="1">
@@ -2589,17 +2588,17 @@
     <row r="1" spans="1:11" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
       <c r="B1" s="26"/>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="37" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>